<commit_message>
pembagian jp per semester
</commit_message>
<xml_diff>
--- a/PEMBAGIAN_JAM_CP.xlsx
+++ b/PEMBAGIAN_JAM_CP.xlsx
@@ -240,50 +240,50 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,10 +565,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B2:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,18 +579,18 @@
     <col min="2" max="2" width="7.33203125" customWidth="1"/>
     <col min="3" max="3" width="116.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -619,13 +622,13 @@
       <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="16">
         <v>3</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="15">
         <v>3</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -639,27 +642,27 @@
       <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="10"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="18">
         <v>3</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="15">
         <v>3</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="12" t="s">
         <v>15</v>
       </c>
     </row>
@@ -667,33 +670,33 @@
       <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="10"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="20">
         <v>6</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="15">
         <v>6</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -701,43 +704,43 @@
       <c r="B9" s="3">
         <v>6</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="19"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>7</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="10"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10">
         <f>SUM(E4:E10)</f>
         <v>12</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="10">
         <f>SUM(F4:F10)</f>
         <v>12</v>
       </c>
-      <c r="G11" s="21"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
@@ -784,6 +787,6 @@
     <mergeCell ref="E8:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>